<commit_message>
First attempt, Forwarding BUG is available, Many unneseccary files are here.
</commit_message>
<xml_diff>
--- a/docs/control_signals/EX_OP_SIG.xlsx
+++ b/docs/control_signals/EX_OP_SIG.xlsx
@@ -228,9 +228,6 @@
     <t>SHAMT</t>
   </si>
   <si>
-    <t>XX</t>
-  </si>
-  <si>
     <t>FUNCT5</t>
   </si>
   <si>
@@ -514,6 +511,9 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>1100</t>
   </si>
 </sst>
 </file>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:V112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1021,7 +1021,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>2</v>
@@ -1048,10 +1048,10 @@
         <v>8</v>
       </c>
       <c r="M4" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1082,25 +1082,25 @@
         <v>9</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>140</v>
+        <v>9</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>164</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1137,19 +1137,19 @@
         <v>16</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1186,19 +1186,19 @@
         <v>16</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -1235,19 +1235,19 @@
         <v>16</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N8" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -1284,29 +1284,29 @@
         <v>16</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -1338,19 +1338,19 @@
         <v>16</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M10" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N10" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P10" s="1"/>
       <c r="Q10" s="4"/>
@@ -1386,19 +1386,19 @@
         <v>16</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N11" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -1435,19 +1435,19 @@
         <v>16</v>
       </c>
       <c r="J12" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -1484,19 +1484,19 @@
         <v>16</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -1533,19 +1533,19 @@
         <v>16</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1582,19 +1582,19 @@
         <v>16</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N15" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1631,19 +1631,19 @@
         <v>16</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N16" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -1680,19 +1680,19 @@
         <v>16</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -1729,19 +1729,19 @@
         <v>16</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -1778,19 +1778,19 @@
         <v>16</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M19" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -1827,19 +1827,19 @@
         <v>16</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M20" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N20" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1876,19 +1876,19 @@
         <v>16</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M21" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N21" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1925,19 +1925,19 @@
         <v>16</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M22" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N22" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1974,19 +1974,19 @@
         <v>16</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L23" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M23" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -2023,19 +2023,19 @@
         <v>59</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L24" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N24" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
@@ -2065,22 +2065,22 @@
         <v>12</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M25" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
@@ -2113,19 +2113,19 @@
         <v>60</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L26" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M26" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N26" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
@@ -2158,19 +2158,19 @@
         <v>65</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M27" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
@@ -2203,19 +2203,19 @@
         <v>61</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M28" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
@@ -2248,19 +2248,19 @@
         <v>62</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M29" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N29" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
@@ -2293,19 +2293,19 @@
         <v>63</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L30" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M30" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N30" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
@@ -2338,19 +2338,19 @@
         <v>64</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L31" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M31" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N31" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
@@ -2359,13 +2359,13 @@
     </row>
     <row r="32" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B32" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>25</v>
@@ -2377,25 +2377,25 @@
         <v>50</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J32" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M32" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N32" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
@@ -2404,13 +2404,13 @@
     </row>
     <row r="33" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>25</v>
@@ -2422,25 +2422,25 @@
         <v>50</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J33" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="M33" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N33" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
@@ -2449,13 +2449,13 @@
     </row>
     <row r="34" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B34" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>25</v>
@@ -2467,25 +2467,25 @@
         <v>50</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I34" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M34" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N34" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
@@ -2494,13 +2494,13 @@
     </row>
     <row r="35" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B35" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>27</v>
@@ -2512,25 +2512,25 @@
         <v>50</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L35" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M35" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N35" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
@@ -2539,13 +2539,13 @@
     </row>
     <row r="36" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B36" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>27</v>
@@ -2557,25 +2557,25 @@
         <v>50</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M36" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N36" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -2588,13 +2588,13 @@
     </row>
     <row r="37" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B37" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>100</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>101</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>25</v>
@@ -2606,36 +2606,36 @@
         <v>50</v>
       </c>
       <c r="H37" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M37" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N37" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B38" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D38" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>103</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>25</v>
@@ -2647,36 +2647,36 @@
         <v>50</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J38" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M38" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N38" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B39" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>27</v>
@@ -2688,36 +2688,36 @@
         <v>50</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J39" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M39" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N39" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B40" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C40" s="11" t="s">
-        <v>107</v>
-      </c>
       <c r="D40" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>25</v>
@@ -2729,36 +2729,36 @@
         <v>50</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J40" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K40" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L40" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M40" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N40" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B41" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E41" s="13" t="s">
         <v>27</v>
@@ -2770,36 +2770,36 @@
         <v>50</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J41" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M41" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N41" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B42" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>25</v>
@@ -2811,36 +2811,36 @@
         <v>50</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J42" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M42" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N42" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B43" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>25</v>
@@ -2852,45 +2852,45 @@
         <v>50</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J43" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M43" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N43" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B44" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>66</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>21</v>
       </c>
       <c r="F44" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H44" s="14" t="s">
         <v>12</v>
@@ -2899,57 +2899,57 @@
         <v>16</v>
       </c>
       <c r="J44" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L44" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M44" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N44" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B45" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>67</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E45" s="14" t="s">
         <v>21</v>
       </c>
       <c r="F45" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H45" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J45" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L45" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M45" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N45" s="9">
         <v>1</v>
@@ -2963,16 +2963,16 @@
         <v>66</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F46" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G46" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H46" s="14" t="s">
         <v>12</v>
@@ -2981,19 +2981,19 @@
         <v>62</v>
       </c>
       <c r="J46" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L46" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M46" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N46" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="2:22" ht="22" x14ac:dyDescent="0.35">
@@ -3004,16 +3004,16 @@
         <v>66</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>40</v>
       </c>
       <c r="F47" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H47" s="14" t="s">
         <v>12</v>
@@ -3022,60 +3022,60 @@
         <v>59</v>
       </c>
       <c r="J47" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L47" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M47" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N47" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="2:22" ht="22" x14ac:dyDescent="0.35">
       <c r="B48" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" s="14" t="s">
         <v>66</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>58</v>
       </c>
       <c r="F48" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H48" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J48" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L48" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M48" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N48" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="2:14" ht="22" x14ac:dyDescent="0.35">
@@ -3086,16 +3086,16 @@
         <v>66</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>26</v>
       </c>
       <c r="F49" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G49" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H49" s="14" t="s">
         <v>12</v>
@@ -3104,19 +3104,19 @@
         <v>60</v>
       </c>
       <c r="J49" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L49" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M49" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N49" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="2:14" ht="22" x14ac:dyDescent="0.35">
@@ -3127,16 +3127,16 @@
         <v>66</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F50" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G50" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H50" s="14" t="s">
         <v>12</v>
@@ -3145,19 +3145,19 @@
         <v>63</v>
       </c>
       <c r="J50" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L50" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M50" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N50" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="2:14" ht="22" x14ac:dyDescent="0.35">
@@ -3168,16 +3168,16 @@
         <v>67</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F51" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G51" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G51" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H51" s="14" t="s">
         <v>12</v>
@@ -3186,19 +3186,19 @@
         <v>64</v>
       </c>
       <c r="J51" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L51" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M51" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N51" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="2:14" ht="22" x14ac:dyDescent="0.35">
@@ -3209,16 +3209,16 @@
         <v>66</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>28</v>
       </c>
       <c r="F52" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G52" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G52" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H52" s="14" t="s">
         <v>12</v>
@@ -3227,19 +3227,19 @@
         <v>65</v>
       </c>
       <c r="J52" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L52" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M52" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N52" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="2:14" ht="22" x14ac:dyDescent="0.35">
@@ -3250,16 +3250,16 @@
         <v>66</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E53" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F53" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G53" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G53" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H53" s="14" t="s">
         <v>12</v>
@@ -3268,839 +3268,839 @@
         <v>61</v>
       </c>
       <c r="J53" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L53" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M53" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N53" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B54" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E54" s="14" t="s">
         <v>21</v>
       </c>
       <c r="F54" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G54" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="H54" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H54" s="14" t="s">
+      <c r="I54" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I54" s="14" t="s">
-        <v>78</v>
-      </c>
       <c r="J54" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K54" s="8" t="s">
         <v>21</v>
       </c>
       <c r="L54" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M54" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N54" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B55" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E55" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F55" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G55" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="H55" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H55" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="I55" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K55" s="8" t="s">
         <v>25</v>
       </c>
       <c r="L55" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M55" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N55" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B56" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E56" s="14" t="s">
         <v>40</v>
       </c>
       <c r="F56" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G56" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G56" s="14" t="s">
+      <c r="H56" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H56" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="I56" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K56" s="8" t="s">
         <v>40</v>
       </c>
       <c r="L56" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M56" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N56" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B57" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E57" s="14" t="s">
         <v>58</v>
       </c>
       <c r="F57" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G57" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G57" s="14" t="s">
+      <c r="H57" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H57" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="I57" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J57" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K57" s="8" t="s">
         <v>58</v>
       </c>
       <c r="L57" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M57" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N57" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="58" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B58" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E58" s="14" t="s">
         <v>26</v>
       </c>
       <c r="F58" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G58" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G58" s="14" t="s">
+      <c r="H58" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H58" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="I58" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J58" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K58" s="8" t="s">
         <v>26</v>
       </c>
       <c r="L58" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M58" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N58" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B59" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E59" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F59" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G59" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G59" s="14" t="s">
+      <c r="H59" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H59" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="I59" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J59" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K59" s="8" t="s">
         <v>27</v>
       </c>
       <c r="L59" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M59" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N59" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B60" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E60" s="14" t="s">
         <v>28</v>
       </c>
       <c r="F60" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G60" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G60" s="14" t="s">
+      <c r="H60" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H60" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="I60" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J60" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K60" s="8" t="s">
         <v>28</v>
       </c>
       <c r="L60" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M60" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N60" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B61" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C61" s="14" t="s">
-        <v>86</v>
-      </c>
       <c r="D61" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E61" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F61" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G61" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G61" s="14" t="s">
+      <c r="H61" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H61" s="14" t="s">
-        <v>77</v>
-      </c>
       <c r="I61" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K61" s="8" t="s">
         <v>29</v>
       </c>
       <c r="L61" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M61" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N61" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B62" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="15" t="s">
-        <v>113</v>
-      </c>
       <c r="D62" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E62" s="14" t="s">
         <v>26</v>
       </c>
       <c r="F62" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G62" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G62" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H62" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="I62" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="I62" s="14" t="s">
-        <v>112</v>
-      </c>
       <c r="J62" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L62" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M62" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N62" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B63" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E63" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F63" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G63" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G63" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H63" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I63" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J63" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K63" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L63" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="M63" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N63" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="2:14" ht="22" x14ac:dyDescent="0.35">
       <c r="B64" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E64" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F64" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G64" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G64" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H64" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I64" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J64" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L64" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M64" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N64" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B65" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E65" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F65" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G65" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G65" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H65" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I65" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K65" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L65" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M65" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N65" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B66" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E66" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F66" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G66" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G66" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H66" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I66" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K66" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M66" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N66" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B67" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E67" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F67" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G67" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G67" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H67" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I67" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J67" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L67" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M67" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N67" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B68" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E68" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F68" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G68" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G68" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H68" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I68" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K68" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L68" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M68" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N68" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B69" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C69" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C69" s="14" t="s">
-        <v>121</v>
-      </c>
       <c r="D69" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E69" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F69" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G69" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G69" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H69" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I69" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J69" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K69" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M69" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N69" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B70" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E70" s="14" t="s">
         <v>28</v>
       </c>
       <c r="F70" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G70" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G70" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H70" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I70" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J70" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M70" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N70" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B71" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E71" s="14" t="s">
         <v>26</v>
       </c>
       <c r="F71" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G71" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G71" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H71" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I71" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J71" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="K71" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="L71" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="K71" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="L71" s="8" t="s">
-        <v>141</v>
-      </c>
       <c r="M71" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N71" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B72" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E72" s="14" t="s">
         <v>27</v>
       </c>
       <c r="F72" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G72" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G72" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="H72" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I72" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J72" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K72" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M72" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N72" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B73" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>67</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E73" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F73" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G73" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G73" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H73" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I73" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J73" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K73" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L73" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M73" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N73" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O73" s="5"/>
       <c r="P73" s="1"/>
@@ -4108,43 +4108,43 @@
     </row>
     <row r="74" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B74" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>67</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E74" s="14" t="s">
         <v>28</v>
       </c>
       <c r="F74" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G74" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G74" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H74" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I74" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J74" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K74" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L74" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M74" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N74" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O74" s="5"/>
       <c r="P74" s="1"/>
@@ -4152,43 +4152,43 @@
     </row>
     <row r="75" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B75" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>67</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E75" s="14" t="s">
         <v>26</v>
       </c>
       <c r="F75" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G75" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G75" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H75" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I75" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J75" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K75" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L75" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M75" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N75" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O75" s="5"/>
       <c r="P75" s="1"/>
@@ -4196,43 +4196,43 @@
     </row>
     <row r="76" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B76" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E76" s="14" t="s">
         <v>40</v>
       </c>
       <c r="F76" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G76" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G76" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H76" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I76" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J76" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K76" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L76" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M76" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N76" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O76" s="5"/>
       <c r="P76" s="1"/>
@@ -4240,43 +4240,43 @@
     </row>
     <row r="77" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B77" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E77" s="14" t="s">
         <v>26</v>
       </c>
       <c r="F77" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G77" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G77" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H77" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I77" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J77" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K77" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L77" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M77" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N77" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O77" s="5"/>
       <c r="P77" s="1"/>
@@ -4284,43 +4284,43 @@
     </row>
     <row r="78" spans="2:17" ht="22" x14ac:dyDescent="0.35">
       <c r="B78" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C78" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="C78" s="14" t="s">
-        <v>160</v>
-      </c>
       <c r="D78" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E78" s="14" t="s">
         <v>28</v>
       </c>
       <c r="F78" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G78" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="G78" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="H78" s="14" t="s">
         <v>12</v>
       </c>
       <c r="I78" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J78" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K78" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L78" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M78" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N78" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O78" s="5"/>
       <c r="P78" s="1"/>

</xml_diff>